<commit_message>
insert Data api completed
</commit_message>
<xml_diff>
--- a/PreviousInvoiceDataBak.xlsx
+++ b/PreviousInvoiceDataBak.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <x:si>
     <x:t>MANOJA_073121</x:t>
   </x:si>
@@ -230,6 +230,9 @@
   </x:si>
   <x:si>
     <x:t>utkarsh.sourcesoft@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>zomatoEng_898ec149-ca86-4fd0-9e42-17d22fd53b12.pdf</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -575,8 +578,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:F16"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="G6" sqref="G6"/>
+    <x:sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <x:selection activeCell="B1" sqref="B1 B:B"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +592,7 @@
     <x:col min="6" max="6" width="30.285156" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -609,7 +612,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -629,7 +632,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -649,7 +652,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
@@ -663,7 +666,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
@@ -680,7 +683,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A6" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -697,7 +700,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A7" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -714,7 +717,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A8" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
@@ -728,7 +731,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A9" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -745,7 +748,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A10" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
@@ -762,7 +765,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A11" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
@@ -779,7 +782,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A12" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
@@ -796,7 +799,7 @@
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A13" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
@@ -813,7 +816,7 @@
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A14" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -830,7 +833,7 @@
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A15" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
@@ -847,7 +850,7 @@
         <x:v>64</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A16" s="0" t="s">
         <x:v>65</x:v>
       </x:c>
@@ -864,265 +867,265 @@
         <x:v>69</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:7">
+    <x:row r="17" spans="1:6">
       <x:c r="A17" s="0" t="s">
-        <x:v>0</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:7">
+    <x:row r="18" spans="1:6">
       <x:c r="A18" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:7">
+    <x:row r="19" spans="1:6">
       <x:c r="A19" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:7">
+    <x:row r="20" spans="1:6">
       <x:c r="A20" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:7">
+    <x:row r="21" spans="1:6">
       <x:c r="A21" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="B21" s="0" t="s">
+      <x:c r="B22" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="D21" s="0" t="s">
+      <x:c r="D22" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="E21" s="0" t="s">
+      <x:c r="E22" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="F21" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:7">
-      <x:c r="A22" s="0" t="s">
+      <x:c r="F22" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B22" s="0" t="s">
+      <x:c r="B23" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D22" s="0" t="s">
+      <x:c r="D23" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="E22" s="0" t="s">
+      <x:c r="E23" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="F22" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:7">
-      <x:c r="A23" s="0" t="s">
+      <x:c r="F23" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B23" s="0" t="s">
+      <x:c r="B24" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="D23" s="0" t="s">
+      <x:c r="D24" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="E23" s="0" t="s">
+      <x:c r="E24" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="F23" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:7">
-      <x:c r="A24" s="0" t="s">
+      <x:c r="F24" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="D24" s="0" t="s">
+      <x:c r="D25" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="E24" s="0" t="s">
+      <x:c r="E25" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="F24" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:7">
-      <x:c r="A25" s="0" t="s">
+      <x:c r="F25" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="B25" s="0" t="s">
+      <x:c r="B26" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="D25" s="0" t="s">
+      <x:c r="D26" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="E25" s="0" t="s">
+      <x:c r="E26" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="F25" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:7">
-      <x:c r="A26" s="0" t="s">
+      <x:c r="F26" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="B26" s="0" t="s">
+      <x:c r="B27" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="D26" s="0" t="s">
+      <x:c r="D27" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="E26" s="0" t="s">
+      <x:c r="E27" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="F26" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:7">
-      <x:c r="A27" s="0" t="s">
+      <x:c r="F27" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="B27" s="0" t="s">
+      <x:c r="B28" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="D27" s="0" t="s">
+      <x:c r="D28" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="E27" s="0" t="s">
+      <x:c r="E28" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="F27" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:7">
-      <x:c r="A28" s="0" t="s">
+      <x:c r="F28" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="B28" s="0" t="s">
+      <x:c r="B29" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="D28" s="0" t="s">
+      <x:c r="D29" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="E28" s="0" t="s">
+      <x:c r="E29" s="0" t="s">
         <x:v>50</x:v>
-      </x:c>
-      <x:c r="F28" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:7">
-      <x:c r="A29" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="D29" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="E29" s="0" t="s">
-        <x:v>55</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="30" spans="1:7">
+    <x:row r="30" spans="1:6">
       <x:c r="A30" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="31" spans="1:7">
+    <x:row r="31" spans="1:6">
       <x:c r="A31" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E31" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F31" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:7">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
       <x:c r="A32" s="0" t="s">
         <x:v>65</x:v>
       </x:c>
@@ -1142,8 +1145,16 @@
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="1" alignWithMargins="1">
+    <x:oddHeader>&amp;LSenderName&amp;CTotalAmount
+&amp;RAttachmentName</x:oddHeader>
+    <x:oddFooter/>
+    <x:evenHeader/>
+    <x:evenFooter/>
+    <x:firstHeader/>
+    <x:firstFooter/>
+  </x:headerFooter>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>